<commit_message>
Fix: Consolidate all CSV outputs to outputs/ directory
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/outputs/optimal_allocations_formatted.xlsx
+++ b/outputs/optimal_allocations_formatted.xlsx
@@ -430,14 +430,14 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="21" customWidth="1" min="2" max="2"/>
-    <col width="9" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="21" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="20" customWidth="1" min="8" max="8"/>
-    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="10" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
@@ -503,10 +503,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0.44135</v>
+        <v>0.4413585586414413</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0.487292</v>
+        <v>0.4872865127134872</v>
       </c>
       <c r="E2" s="3" t="n">
         <v>0</v>
@@ -515,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>0.021358</v>
+        <v>0.02135497864502135</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>0</v>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>0.05</v>
+        <v>0.04999995000005</v>
       </c>
     </row>
     <row r="3">
@@ -568,19 +568,19 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.5030965030965031</v>
+        <v>0.5030945030945031</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.03495103495103496</v>
+        <v>0.03496003496003496</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0.4119524119524119</v>
+        <v>0.4119454119454119</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>0</v>
@@ -592,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>0.05000005000005001</v>
+        <v>0.05000005000005</v>
       </c>
     </row>
     <row r="5">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.4644304644304644</v>
+        <v>0.46443</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>0</v>
@@ -620,13 +620,13 @@
         <v>0</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>0.0810950810950811</v>
+        <v>0.081109</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>0.4044744044744044</v>
+        <v>0.404461</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>0.05000005000005</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="6">

</xml_diff>